<commit_message>
Added hyperoxemia and hypocapnia events. Tweaked mechanical ventilator ARDS validation matrix.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_multiplex_ventilation\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D0E8B3-453A-4E1A-8420-722B912D644C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A93F318-32F6-4627-BBD8-48E35FDCC787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4695" yWindow="2370" windowWidth="39090" windowHeight="20520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="51">
   <si>
     <t>Description</t>
   </si>
@@ -142,16 +142,7 @@
     <t>&gt;20% @cite radermacher2017fifty</t>
   </si>
   <si>
-    <t>&gt;1% @cite radermacher2017fifty</t>
-  </si>
-  <si>
     <t>20 (ventilator setting)</t>
-  </si>
-  <si>
-    <t>21 (ventilator setting)</t>
-  </si>
-  <si>
-    <t>22 (ventilator setting)</t>
   </si>
   <si>
     <t>88%-95% @cite mortelliti2002acute (ventilator target)</t>
@@ -198,6 +189,9 @@
   <si>
     <t>Use apnea to mimic neuromuscular blockade
 Ventilator settings chosen for target tidal volume and oxygen saturation</t>
+  </si>
+  <si>
+    <t>2%-5% @cite Levitzky2013pulmonary</t>
   </si>
 </sst>
 </file>
@@ -1291,13 +1285,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>9</v>
@@ -1391,8 +1385,8 @@
   </sheetPr>
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1450,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>8</v>
@@ -1480,7 +1474,7 @@
         <v>8</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="U1" s="11" t="s">
         <v>8</v>
@@ -1578,7 +1572,7 @@
         <v>9</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>10</v>
@@ -1590,25 +1584,25 @@
         <v>10</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="S3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="U3" s="11" t="s">
         <v>11</v>
@@ -1641,7 +1635,7 @@
         <v>9</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>10</v>
@@ -1653,25 +1647,25 @@
         <v>10</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="O4" s="16" t="s">
         <v>10</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Q4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="S4" s="16" t="s">
         <v>10</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="U4" s="11" t="s">
         <v>11</v>
@@ -1688,7 +1682,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>8</v>
@@ -1706,7 +1700,7 @@
         <v>9</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>10</v>
@@ -1718,25 +1712,25 @@
         <v>10</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="O5" s="16" t="s">
         <v>10</v>
       </c>
       <c r="P5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="T5" s="13" t="s">
-        <v>41</v>
       </c>
       <c r="U5" s="11" t="s">
         <v>11</v>
@@ -1771,7 +1765,7 @@
         <v>9</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>10</v>
@@ -1789,19 +1783,19 @@
         <v>10</v>
       </c>
       <c r="P6" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Q6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="R6" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="S6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="T6" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="U6" s="11" t="s">
         <v>11</v>
@@ -1836,7 +1830,7 @@
         <v>9</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K7" s="11" t="s">
         <v>10</v>
@@ -1854,19 +1848,19 @@
         <v>10</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="11" t="s">
         <v>10</v>
       </c>
       <c r="R7" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="S7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="U7" s="11" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Forgot to save excel file before last commit.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_multiplex_ventilation\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A93F318-32F6-4627-BBD8-48E35FDCC787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230E6F2F-EA6E-4FEF-934F-C3AEFDB8CEEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1385,8 +1385,8 @@
   </sheetPr>
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Mechanical Ventilator methodology report.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_multiplex_ventilation\source\data\human\adult\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_3x\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230E6F2F-EA6E-4FEF-934F-C3AEFDB8CEEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C32998-9144-4EBF-A03A-87A624B4B15E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -106,18 +106,6 @@
     <t>Ventilator settings chosen for target tidal volume and oxygen saturation</t>
   </si>
   <si>
-    <t>Apnea (Dyspnea severity = 1.0)
-Turn on P-CMV mechanical ventilator and provide supplemental oxygen</t>
-  </si>
-  <si>
-    <t>Moderate ARDS (severity = 0.3)
-Adjust ventilator settings</t>
-  </si>
-  <si>
-    <t>Severe ARDS (severity = 0.9)
-Adjust ventilator settings</t>
-  </si>
-  <si>
     <t>Ventilator settings chosen for target tidal volume and supplemental oxygen at max (1.0 fraction O2)</t>
   </si>
   <si>
@@ -187,11 +175,19 @@
     <t>Reduced  further  (artificial airway) @cite mortelliti2002acute @cite arnal2018parameters</t>
   </si>
   <si>
-    <t>Use apnea to mimic neuromuscular blockade
-Ventilator settings chosen for target tidal volume and oxygen saturation</t>
-  </si>
-  <si>
     <t>2%-5% @cite Levitzky2013pulmonary</t>
+  </si>
+  <si>
+    <t>Apnea (Dyspnea severity = 1.0); Turn on P-CMV mechanical ventilator and provide supplemental oxygen</t>
+  </si>
+  <si>
+    <t>Moderate ARDS (severity = 0.3); Adjust ventilator settings</t>
+  </si>
+  <si>
+    <t>Severe ARDS (severity = 0.9); Adjust ventilator settings</t>
+  </si>
+  <si>
+    <t>Use apnea to mimic neuromuscular blockade; Ventilator settings chosen for target tidal volume and oxygen saturation</t>
   </si>
 </sst>
 </file>
@@ -1285,13 +1281,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>9</v>
@@ -1385,8 +1381,8 @@
   </sheetPr>
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,13 +1446,13 @@
         <v>8</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>8</v>
@@ -1474,7 +1470,7 @@
         <v>8</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="U1" s="11" t="s">
         <v>8</v>
@@ -1556,7 +1552,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>8</v>
@@ -1572,37 +1568,37 @@
         <v>9</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="S3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="U3" s="11" t="s">
         <v>11</v>
@@ -1635,54 +1631,54 @@
         <v>9</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M4" s="16" t="s">
         <v>10</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="O4" s="16" t="s">
         <v>10</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Q4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="S4" s="16" t="s">
         <v>10</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="U4" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>8</v>
@@ -1700,37 +1696,37 @@
         <v>9</v>
       </c>
       <c r="J5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="P5" s="7" t="s">
+      <c r="S5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="T5" s="13" t="s">
-        <v>38</v>
       </c>
       <c r="U5" s="11" t="s">
         <v>11</v>
@@ -1741,7 +1737,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>8</v>
@@ -1765,37 +1761,37 @@
         <v>9</v>
       </c>
       <c r="J6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="P6" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="R6" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="S6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="T6" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="U6" s="11" t="s">
         <v>11</v>
@@ -1806,13 +1802,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>8</v>
@@ -1830,37 +1826,37 @@
         <v>9</v>
       </c>
       <c r="J7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="P7" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="R7" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="S7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="U7" s="11" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Typo fixes in mechanical ventilator documentation.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_3x\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C32998-9144-4EBF-A03A-87A624B4B15E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBB9F1F-841F-4BAA-AB50-DF52860D9BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31755" yWindow="2955" windowWidth="24210" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -181,13 +181,13 @@
     <t>Apnea (Dyspnea severity = 1.0); Turn on P-CMV mechanical ventilator and provide supplemental oxygen</t>
   </si>
   <si>
-    <t>Moderate ARDS (severity = 0.3); Adjust ventilator settings</t>
-  </si>
-  <si>
     <t>Severe ARDS (severity = 0.9); Adjust ventilator settings</t>
   </si>
   <si>
     <t>Use apnea to mimic neuromuscular blockade; Ventilator settings chosen for target tidal volume and oxygen saturation</t>
+  </si>
+  <si>
+    <t>Moderate ARDS (severity = 0.6); Adjust ventilator settings</t>
   </si>
 </sst>
 </file>
@@ -1382,7 +1382,7 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,7 +1678,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>8</v>
@@ -1737,7 +1737,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>8</v>
@@ -1802,7 +1802,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>8</v>

</xml_diff>